<commit_message>
Fixed bug in loads and compile no-fiber loads
</commit_message>
<xml_diff>
--- a/loads/plastic_loads-7classes-v03.xlsx
+++ b/loads/plastic_loads-7classes-v03.xlsx
@@ -485,22 +485,22 @@
         <v>0.01745650183150183</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03491300366300366</v>
+        <v>0.03250201727728265</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01187042124542125</v>
+        <v>0.01057098089511844</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01396520146520147</v>
+        <v>0.009783109047814931</v>
       </c>
       <c r="G4" t="n">
-        <v>0.006982600732600733</v>
+        <v>0.00551796997783287</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002793040293040293</v>
+        <v>0.002081935221641104</v>
       </c>
       <c r="I4" t="n">
         <v>0.01745650183150183</v>
@@ -531,25 +531,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.006716380654501717</v>
+        <v>0.006716380654501716</v>
       </c>
       <c r="C5" t="n">
-        <v>0.007233025320232618</v>
+        <v>0.006011865201232306</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007233025320232618</v>
+        <v>0.005823994413693795</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.01033289331461803</v>
+        <v>0.008760496505871806</v>
       </c>
       <c r="G5" t="n">
-        <v>0.004649801991578112</v>
+        <v>0.003317348851699008</v>
       </c>
       <c r="H5" t="n">
-        <v>0.001549933997192704</v>
+        <v>0.001127224725231057</v>
       </c>
       <c r="I5" t="n">
         <v>0.006716380654501716</v>
@@ -583,22 +583,22 @@
         <v>0.01524390243902439</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05235949098621421</v>
+        <v>0.04984916043789812</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01126723223753977</v>
+        <v>0.009346932555129099</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01458112407211029</v>
+        <v>0.01004477436078708</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01193001060445387</v>
+        <v>0.008996506053690729</v>
       </c>
       <c r="H6" t="n">
-        <v>0.001325556733828208</v>
+        <v>0.001182682355331754</v>
       </c>
       <c r="I6" t="n">
         <v>0.01524390243902439</v>
@@ -632,22 +632,22 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001407129455909944</v>
+        <v>0.001294559099437148</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004690431519699813</v>
+        <v>0.000260749703258414</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00375234521575985</v>
+        <v>0.001468308997471246</v>
       </c>
       <c r="G7" t="n">
-        <v>0.003048780487804878</v>
+        <v>0.001562209189083905</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0004690431519699813</v>
+        <v>0.0002439024390243902</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -681,22 +681,22 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0006981020350920934</v>
+        <v>0.0004238476641630567</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0003490510175460467</v>
+        <v>9.972886215601335e-05</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003839561193006514</v>
+        <v>0.002576104324475938</v>
       </c>
       <c r="G8" t="n">
-        <v>0.004537663228098607</v>
+        <v>0.002865857099658951</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0001745255087730234</v>
+        <v>9.972886215601333e-05</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -727,25 +727,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02717627707764737</v>
+        <v>0.02802616165560328</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09058759025882458</v>
+        <v>0.09250247053135975</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02616974829699376</v>
+        <v>0.0261401247382887</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02616974829699376</v>
+        <v>0.02015516028062719</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02315016195503295</v>
+        <v>0.01360349367621611</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001006528780653606</v>
+        <v>0.0009161436491194176</v>
       </c>
       <c r="I9" t="n">
         <v>0.02802616165560328</v>
@@ -776,22 +776,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.004212282809935967</v>
+        <v>0.004139342847859153</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01143333905554048</v>
+        <v>0.01097337072326017</v>
       </c>
       <c r="D10" t="n">
-        <v>0.002407018748534838</v>
+        <v>0.002329613074494138</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0009026320307005642</v>
+        <v>0.0007932220875853444</v>
       </c>
       <c r="F10" t="n">
-        <v>0.003911405466369111</v>
+        <v>0.002144964288008869</v>
       </c>
       <c r="G10" t="n">
-        <v>0.003008773435668547</v>
+        <v>0.002241967474901839</v>
       </c>
       <c r="H10" t="n">
         <v>0.0003008773435668548</v>
@@ -825,22 +825,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0009920634920634922</v>
+        <v>0.000992063492063492</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0009920634920634922</v>
+        <v>0.0003306878306878307</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001984126984126984</v>
+        <v>0.0006613756613756613</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.01190476190476191</v>
+        <v>0.005304101838755305</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01190476190476191</v>
+        <v>0.005081460527005081</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>

</xml_diff>